<commit_message>
updated calendar and news for lab02a
</commit_message>
<xml_diff>
--- a/CS320-Spring2017Calendar.xlsx
+++ b/CS320-Spring2017Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Monday</t>
   </si>
@@ -136,10 +136,6 @@
 (in-class session)</t>
   </si>
   <si>
-    <t>A05: Use Cases due
-(Google Doc)</t>
-  </si>
-  <si>
     <t>A06: Team Problem Domain Analysis due
 (Violet UML &amp; Google Doc)</t>
   </si>
@@ -269,23 +265,25 @@
 Development Process discussion</t>
   </si>
   <si>
+    <t>Lab 2: Web Applications
+(in class)</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 A01: Team Project Proposal due
 (Google Doc)
- Lab 2: Web Applications Due (Marmoset)
+ Lab 2: Web Applications I Due (Marmoset)
 </t>
   </si>
   <si>
-    <t>Lab 2: Web Applications
-(in class)</t>
+    <t>Lab 2a: Web Applications II Due
+(Marmoset)
+A05: Use Cases due
+(Google Doc)</t>
   </si>
   <si>
     <t>CS320: SW Engineering - Spring 2017 Schedule
-(as of 1-22-2017, subject to change)</t>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2017 Schedule
-(as of 1-22-17, subject to change)</t>
+(as of 1-26-2017, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -955,6 +953,42 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -967,55 +1001,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1319,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:I30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,27 +1338,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="63"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="75"/>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -1378,14 +1376,14 @@
         <v>4</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="72">
+      <c r="B3" s="80">
         <v>1</v>
       </c>
       <c r="C3" s="5">
@@ -1417,29 +1415,29 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
-      <c r="B4" s="68"/>
+      <c r="A4" s="79"/>
+      <c r="B4" s="64"/>
       <c r="C4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="68">
+      <c r="A5" s="79"/>
+      <c r="B5" s="64">
         <f>B3 + 1</f>
         <v>2</v>
       </c>
@@ -1473,27 +1471,27 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="70"/>
-      <c r="B6" s="68"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70"/>
-      <c r="B7" s="68">
+      <c r="A7" s="79"/>
+      <c r="B7" s="64">
         <f>B5 + 1</f>
         <v>3</v>
       </c>
@@ -1526,29 +1524,29 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="144.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" s="73"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" s="21"/>
-      <c r="F8" s="81" t="s">
-        <v>33</v>
+      <c r="F8" s="61" t="s">
+        <v>32</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I8" s="25"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="77">
+      <c r="A9" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="66">
         <f>B7 + 1</f>
         <v>4</v>
       </c>
@@ -1582,10 +1580,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="A10" s="75"/>
-      <c r="B10" s="74"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>20</v>
@@ -1601,8 +1599,8 @@
       <c r="I10" s="25"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="74">
+      <c r="A11" s="81"/>
+      <c r="B11" s="67">
         <f>B9 + 1</f>
         <v>5</v>
       </c>
@@ -1635,11 +1633,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="A12" s="75"/>
-      <c r="B12" s="74"/>
+    <row r="12" spans="1:9" ht="96" x14ac:dyDescent="0.25">
+      <c r="A12" s="81"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="30" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>21</v>
@@ -1655,8 +1653,8 @@
       <c r="I12" s="25"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="75"/>
-      <c r="B13" s="74">
+      <c r="A13" s="81"/>
+      <c r="B13" s="67">
         <f>B11 + 1</f>
         <v>6</v>
       </c>
@@ -1690,31 +1688,31 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="75"/>
-      <c r="B14" s="74"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="67"/>
       <c r="C14" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="75"/>
-      <c r="B15" s="74">
+      <c r="A15" s="81"/>
+      <c r="B15" s="67">
         <f>B13 + 1</f>
         <v>7</v>
       </c>
@@ -1747,8 +1745,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="67"/>
-      <c r="B16" s="65"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="68"/>
       <c r="C16" s="34" t="str">
         <f>I14</f>
         <v>WINTER BREAK</v>
@@ -1844,29 +1842,29 @@
       <c r="H22" s="57"/>
       <c r="I22" s="57"/>
     </row>
-    <row r="23" spans="1:9" s="58" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="54"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
-    </row>
-    <row r="24" spans="1:9" s="58" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
-    </row>
-    <row r="25" spans="1:9" s="58" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+    </row>
+    <row r="24" spans="1:9" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+    </row>
+    <row r="25" spans="1:9" s="58" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="54"/>
       <c r="B25" s="54"/>
       <c r="C25" s="57"/>
@@ -1877,425 +1875,497 @@
       <c r="H25" s="57"/>
       <c r="I25" s="57"/>
     </row>
-    <row r="26" spans="1:9" s="58" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-    </row>
-    <row r="27" spans="1:9" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-    </row>
-    <row r="28" spans="1:9" s="56" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-    </row>
-    <row r="29" spans="1:9" s="58" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
-    </row>
-    <row r="30" spans="1:9" s="55" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="63"/>
-    </row>
-    <row r="31" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="26" spans="1:9" s="55" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="73" t="str">
+        <f>A1</f>
+        <v>CS320: SW Engineering - Spring 2017 Schedule
+(as of 1-26-2017, subject to change)</v>
+      </c>
+      <c r="B26" s="74"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="75"/>
+    </row>
+    <row r="27" spans="1:9" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="64">
+    </row>
+    <row r="28" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="77" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="76">
         <f>B15</f>
         <v>7</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C28" s="9">
         <f>C15</f>
         <v>26</v>
       </c>
-      <c r="D32" s="10">
-        <f>C32 + 1</f>
+      <c r="D28" s="10">
+        <f>C28 + 1</f>
         <v>27</v>
       </c>
-      <c r="E32" s="31">
-        <f t="shared" ref="E32" si="3">D32 + 1</f>
+      <c r="E28" s="31">
+        <f t="shared" ref="E28" si="3">D28 + 1</f>
         <v>28</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F28" s="32">
         <f>F15</f>
         <v>1</v>
       </c>
-      <c r="G32" s="6">
-        <f>F32 + 1</f>
+      <c r="G28" s="6">
+        <f>F28 + 1</f>
         <v>2</v>
       </c>
-      <c r="H32" s="6">
-        <f>G32 + 1</f>
+      <c r="H28" s="6">
+        <f>G28 + 1</f>
         <v>3</v>
       </c>
-      <c r="I32" s="33">
-        <f>H32 + 1</f>
+      <c r="I28" s="33">
+        <f>H28 + 1</f>
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="67"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="34" t="str">
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="78"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="34" t="str">
         <f>C16</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="D33" s="34" t="str">
-        <f t="shared" ref="D33" si="4">C33</f>
+      <c r="D29" s="34" t="str">
+        <f t="shared" ref="D29" si="4">C29</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="E33" s="35" t="str">
-        <f t="shared" ref="E33" si="5">D33</f>
+      <c r="E29" s="35" t="str">
+        <f t="shared" ref="E29" si="5">D29</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="F33" s="9" t="str">
-        <f>E33</f>
+      <c r="F29" s="9" t="str">
+        <f>E29</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="G33" s="10" t="str">
-        <f>F33</f>
+      <c r="G29" s="10" t="str">
+        <f>F29</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="H33" s="10" t="str">
-        <f>G33</f>
+      <c r="H29" s="10" t="str">
+        <f>G29</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="I33" s="31" t="str">
-        <f t="shared" ref="I33" si="6">H33</f>
+      <c r="I29" s="31" t="str">
+        <f t="shared" ref="I29" si="6">H29</f>
         <v>WINTER BREAK</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="69" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="76">
-        <f>B32 + 1</f>
+    <row r="30" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="69">
+        <f>B28 + 1</f>
         <v>8</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C30" s="9">
         <f>I15 + 1</f>
         <v>5</v>
       </c>
+      <c r="D30" s="11">
+        <f>C30 + 1</f>
+        <v>6</v>
+      </c>
+      <c r="E30" s="11">
+        <f t="shared" ref="E30:I30" si="7">D30 + 1</f>
+        <v>7</v>
+      </c>
+      <c r="F30" s="36">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="G30" s="36">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="H30" s="36">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="I30" s="37">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="108" x14ac:dyDescent="0.25">
+      <c r="A31" s="79"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="79"/>
+      <c r="B32" s="64">
+        <f>B30 + 1</f>
+        <v>9</v>
+      </c>
+      <c r="C32" s="39">
+        <f>I30 + 1</f>
+        <v>12</v>
+      </c>
+      <c r="D32" s="11">
+        <f>C32 + 1</f>
+        <v>13</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" ref="E32:I32" si="8">D32 + 1</f>
+        <v>14</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="G32" s="11">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="H32" s="11">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="I32" s="15">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+      <c r="A33" s="79"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="79"/>
+      <c r="B34" s="64">
+        <f>B32 + 1</f>
+        <v>10</v>
+      </c>
+      <c r="C34" s="14">
+        <f>I32 + 1</f>
+        <v>19</v>
+      </c>
       <c r="D34" s="11">
         <f>C34 + 1</f>
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E34" s="11">
-        <f t="shared" ref="E34:I34" si="7">D34 + 1</f>
+        <f t="shared" ref="E34:I36" si="9">D34 + 1</f>
+        <v>21</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="G34" s="11">
+        <f t="shared" si="9"/>
+        <v>23</v>
+      </c>
+      <c r="H34" s="11">
+        <f t="shared" si="9"/>
+        <v>24</v>
+      </c>
+      <c r="I34" s="15">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="79"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="36">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="G34" s="36">
-        <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-      <c r="H34" s="36">
-        <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="I34" s="37">
-        <f t="shared" si="7"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="12"/>
+      <c r="H35" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="79"/>
+      <c r="B36" s="64">
+        <f>B34 + 1</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="108" x14ac:dyDescent="0.25">
-      <c r="A35" s="70"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I35" s="13"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="70"/>
-      <c r="B36" s="68">
-        <f>B34 + 1</f>
-        <v>9</v>
-      </c>
-      <c r="C36" s="39">
+      <c r="C36" s="14">
         <f>I34 + 1</f>
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D36" s="11">
         <f>C36 + 1</f>
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E36" s="11">
-        <f t="shared" ref="E36:I36" si="8">D36 + 1</f>
-        <v>14</v>
-      </c>
-      <c r="F36" s="11">
-        <f t="shared" si="8"/>
-        <v>15</v>
-      </c>
-      <c r="G36" s="11">
-        <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-      <c r="H36" s="11">
-        <f t="shared" si="8"/>
-        <v>17</v>
-      </c>
-      <c r="I36" s="15">
-        <f t="shared" si="8"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="A37" s="70"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I37" s="13"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="70"/>
-      <c r="B38" s="68">
-        <f>B36 + 1</f>
-        <v>10</v>
-      </c>
-      <c r="C38" s="14">
-        <f>I36 + 1</f>
-        <v>19</v>
-      </c>
-      <c r="D38" s="11">
-        <f>C38 + 1</f>
-        <v>20</v>
-      </c>
-      <c r="E38" s="11">
-        <f t="shared" ref="E38:I40" si="9">D38 + 1</f>
-        <v>21</v>
-      </c>
-      <c r="F38" s="11">
-        <f t="shared" si="9"/>
-        <v>22</v>
-      </c>
-      <c r="G38" s="11">
-        <f t="shared" si="9"/>
-        <v>23</v>
-      </c>
-      <c r="H38" s="11">
-        <f t="shared" si="9"/>
-        <v>24</v>
-      </c>
-      <c r="I38" s="15">
-        <f t="shared" si="9"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="70"/>
-      <c r="B39" s="68"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="70"/>
-      <c r="B40" s="68">
-        <f>B38 + 1</f>
-        <v>11</v>
-      </c>
-      <c r="C40" s="14">
-        <f>I38 + 1</f>
-        <v>26</v>
-      </c>
-      <c r="D40" s="11">
-        <f>C40 + 1</f>
-        <v>27</v>
-      </c>
-      <c r="E40" s="11">
         <f t="shared" si="9"/>
         <v>28</v>
       </c>
-      <c r="F40" s="11">
+      <c r="F36" s="11">
         <f t="shared" si="9"/>
         <v>29</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G36" s="11">
         <f t="shared" si="9"/>
         <v>30</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H36" s="15">
         <f t="shared" si="9"/>
         <v>31</v>
       </c>
-      <c r="I40" s="41">
+      <c r="I36" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="71"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="20" t="s">
+    <row r="37" spans="1:9" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="63"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="43"/>
-      <c r="F41" s="20" t="s">
+      <c r="E37" s="43"/>
+      <c r="F37" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="43"/>
-      <c r="H41" s="44" t="s">
+      <c r="G37" s="43"/>
+      <c r="H37" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="I41" s="45"/>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="78" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="77">
-        <f>B40 + 1</f>
+      <c r="I37" s="45"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="66">
+        <f>B36 + 1</f>
         <v>12</v>
       </c>
-      <c r="C42" s="30">
-        <f>I40 + 1</f>
+      <c r="C38" s="30">
+        <f>I36 + 1</f>
         <v>2</v>
       </c>
-      <c r="D42" s="27">
-        <f>C42 + 1</f>
+      <c r="D38" s="27">
+        <f>C38 + 1</f>
         <v>3</v>
       </c>
-      <c r="E42" s="24">
-        <f t="shared" ref="E42:I42" si="10">D42 + 1</f>
+      <c r="E38" s="24">
+        <f t="shared" ref="E38:I38" si="10">D38 + 1</f>
         <v>4</v>
       </c>
-      <c r="F42" s="24">
+      <c r="F38" s="24">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="G42" s="24">
+      <c r="G38" s="24">
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="H42" s="27">
+      <c r="H38" s="27">
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="I42" s="28">
+      <c r="I38" s="28">
         <f t="shared" si="10"/>
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="A43" s="79"/>
-      <c r="B43" s="74"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="46" t="s">
+    <row r="39" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+      <c r="A39" s="71"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="46" t="s">
         <v>9</v>
+      </c>
+      <c r="E39" s="23"/>
+      <c r="F39" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="23"/>
+      <c r="H39" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" s="25"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="71"/>
+      <c r="B40" s="67">
+        <f>B38 + 1</f>
+        <v>13</v>
+      </c>
+      <c r="C40" s="30">
+        <f>I38 + 1</f>
+        <v>9</v>
+      </c>
+      <c r="D40" s="27">
+        <f>C40 + 1</f>
+        <v>10</v>
+      </c>
+      <c r="E40" s="24">
+        <f t="shared" ref="E40:I40" si="11">D40 + 1</f>
+        <v>11</v>
+      </c>
+      <c r="F40" s="24">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="G40" s="10">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="H40" s="10">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="I40" s="31">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="48" x14ac:dyDescent="0.25">
+      <c r="A41" s="71"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="23"/>
+      <c r="F41" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H41" s="10" t="str">
+        <f>G41</f>
+        <v>SPRING BREAK</v>
+      </c>
+      <c r="I41" s="31" t="str">
+        <f>H41</f>
+        <v>SPRING BREAK</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="71"/>
+      <c r="B42" s="67">
+        <f>B40 + 1</f>
+        <v>14</v>
+      </c>
+      <c r="C42" s="9">
+        <f>I40 + 1</f>
+        <v>16</v>
+      </c>
+      <c r="D42" s="10">
+        <f>C42 + 1</f>
+        <v>17</v>
+      </c>
+      <c r="E42" s="24">
+        <f t="shared" ref="E42:I44" si="12">D42 + 1</f>
+        <v>18</v>
+      </c>
+      <c r="F42" s="24">
+        <f t="shared" si="12"/>
+        <v>19</v>
+      </c>
+      <c r="G42" s="24">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="H42" s="24">
+        <f t="shared" si="12"/>
+        <v>21</v>
+      </c>
+      <c r="I42" s="28">
+        <f t="shared" si="12"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="71"/>
+      <c r="B43" s="67"/>
+      <c r="C43" s="9" t="str">
+        <f>I41</f>
+        <v>SPRING BREAK</v>
+      </c>
+      <c r="D43" s="10" t="str">
+        <f>C43</f>
+        <v>SPRING BREAK</v>
       </c>
       <c r="E43" s="23"/>
       <c r="F43" s="24" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="G43" s="23"/>
       <c r="H43" s="46" t="s">
@@ -2304,295 +2374,171 @@
       <c r="I43" s="25"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="79"/>
-      <c r="B44" s="74">
+      <c r="A44" s="71"/>
+      <c r="B44" s="67">
         <f>B42 + 1</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C44" s="30">
         <f>I42 + 1</f>
-        <v>9</v>
-      </c>
-      <c r="D44" s="27">
+        <v>23</v>
+      </c>
+      <c r="D44" s="24">
         <f>C44 + 1</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E44" s="24">
-        <f t="shared" ref="E44:I44" si="11">D44 + 1</f>
-        <v>11</v>
+        <f t="shared" si="12"/>
+        <v>25</v>
       </c>
       <c r="F44" s="24">
-        <f t="shared" si="11"/>
-        <v>12</v>
-      </c>
-      <c r="G44" s="10">
-        <f t="shared" si="11"/>
-        <v>13</v>
-      </c>
-      <c r="H44" s="10">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
-      <c r="I44" s="31">
-        <f t="shared" si="11"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="48" x14ac:dyDescent="0.25">
-      <c r="A45" s="79"/>
-      <c r="B45" s="74"/>
+        <f t="shared" si="12"/>
+        <v>26</v>
+      </c>
+      <c r="G44" s="24">
+        <f t="shared" si="12"/>
+        <v>27</v>
+      </c>
+      <c r="H44" s="24">
+        <f t="shared" si="12"/>
+        <v>28</v>
+      </c>
+      <c r="I44" s="28">
+        <f t="shared" si="12"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="71"/>
+      <c r="B45" s="67"/>
       <c r="C45" s="29"/>
       <c r="D45" s="24" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E45" s="23"/>
       <c r="F45" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H45" s="10" t="str">
-        <f>G45</f>
-        <v>SPRING BREAK</v>
-      </c>
-      <c r="I45" s="31" t="str">
-        <f>H45</f>
-        <v>SPRING BREAK</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="79"/>
-      <c r="B46" s="74">
+        <v>25</v>
+      </c>
+      <c r="G45" s="23"/>
+      <c r="H45" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" s="25"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="71"/>
+      <c r="B46" s="67">
         <f>B44 + 1</f>
-        <v>14</v>
-      </c>
-      <c r="C46" s="9">
+        <v>16</v>
+      </c>
+      <c r="C46" s="47">
         <f>I44 + 1</f>
-        <v>16</v>
-      </c>
-      <c r="D46" s="10">
-        <f>C46 + 1</f>
+        <v>30</v>
+      </c>
+      <c r="D46" s="48">
+        <v>1</v>
+      </c>
+      <c r="E46" s="7">
+        <f>D46 + 1</f>
+        <v>2</v>
+      </c>
+      <c r="F46" s="49">
+        <f>E46 + 1</f>
+        <v>3</v>
+      </c>
+      <c r="G46" s="7">
+        <f>F46 + 1</f>
+        <v>4</v>
+      </c>
+      <c r="H46" s="7">
+        <f>G46 + 1</f>
+        <v>5</v>
+      </c>
+      <c r="I46" s="8">
+        <f>H46 + 1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="72"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="12"/>
+      <c r="F47" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47" s="12"/>
+      <c r="H47" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I47" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="69">
+        <f>B46 + 1</f>
         <v>17</v>
       </c>
-      <c r="E46" s="24">
-        <f t="shared" ref="E46:I48" si="12">D46 + 1</f>
-        <v>18</v>
-      </c>
-      <c r="F46" s="24">
-        <f t="shared" si="12"/>
-        <v>19</v>
-      </c>
-      <c r="G46" s="24">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H46" s="24">
-        <f t="shared" si="12"/>
-        <v>21</v>
-      </c>
-      <c r="I46" s="28">
-        <f t="shared" si="12"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="79"/>
-      <c r="B47" s="74"/>
-      <c r="C47" s="9" t="str">
-        <f>I45</f>
-        <v>SPRING BREAK</v>
-      </c>
-      <c r="D47" s="10" t="str">
-        <f>C47</f>
-        <v>SPRING BREAK</v>
-      </c>
-      <c r="E47" s="23"/>
-      <c r="F47" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="23"/>
-      <c r="H47" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="I47" s="25"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="79"/>
-      <c r="B48" s="74">
-        <f>B46 + 1</f>
-        <v>15</v>
-      </c>
-      <c r="C48" s="30">
+      <c r="C48" s="14">
         <f>I46 + 1</f>
-        <v>23</v>
-      </c>
-      <c r="D48" s="24">
+        <v>7</v>
+      </c>
+      <c r="D48" s="11">
         <f>C48 + 1</f>
-        <v>24</v>
-      </c>
-      <c r="E48" s="24">
-        <f t="shared" si="12"/>
-        <v>25</v>
-      </c>
-      <c r="F48" s="24">
-        <f t="shared" si="12"/>
-        <v>26</v>
-      </c>
-      <c r="G48" s="24">
-        <f t="shared" si="12"/>
-        <v>27</v>
-      </c>
-      <c r="H48" s="24">
-        <f t="shared" si="12"/>
-        <v>28</v>
-      </c>
-      <c r="I48" s="28">
-        <f t="shared" si="12"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="79"/>
-      <c r="B49" s="74"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="23"/>
-      <c r="H49" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="I49" s="25"/>
-    </row>
-    <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="79"/>
-      <c r="B50" s="74">
-        <f>B48 + 1</f>
-        <v>16</v>
-      </c>
-      <c r="C50" s="47">
-        <f>I48 + 1</f>
-        <v>30</v>
-      </c>
-      <c r="D50" s="48">
-        <v>1</v>
-      </c>
-      <c r="E50" s="7">
-        <f>D50 + 1</f>
-        <v>2</v>
-      </c>
-      <c r="F50" s="49">
-        <f>E50 + 1</f>
-        <v>3</v>
-      </c>
-      <c r="G50" s="7">
-        <f>F50 + 1</f>
-        <v>4</v>
-      </c>
-      <c r="H50" s="7">
-        <f>G50 + 1</f>
-        <v>5</v>
-      </c>
-      <c r="I50" s="8">
-        <f>H50 + 1</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="80"/>
-      <c r="B51" s="65"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="12"/>
-      <c r="F51" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="G51" s="12"/>
-      <c r="H51" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="69" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="76">
-        <f>B50 + 1</f>
-        <v>17</v>
-      </c>
-      <c r="C52" s="14">
-        <f>I50 + 1</f>
-        <v>7</v>
-      </c>
-      <c r="D52" s="11">
-        <f>C52 + 1</f>
         <v>8</v>
       </c>
-      <c r="E52" s="11">
-        <f t="shared" ref="E52:I52" si="13">D52 + 1</f>
+      <c r="E48" s="11">
+        <f t="shared" ref="E48:I48" si="13">D48 + 1</f>
         <v>9</v>
       </c>
-      <c r="F52" s="51">
+      <c r="F48" s="51">
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G48" s="11">
         <f t="shared" si="13"/>
         <v>11</v>
       </c>
-      <c r="H52" s="11">
+      <c r="H48" s="11">
         <f t="shared" si="13"/>
         <v>12</v>
       </c>
-      <c r="I52" s="15">
+      <c r="I48" s="15">
         <f t="shared" si="13"/>
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="71"/>
-      <c r="B53" s="73"/>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="F53" s="52" t="s">
+    <row r="49" spans="1:9" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="63"/>
+      <c r="B49" s="65"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G53" s="43"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="21"/>
-    </row>
-    <row r="54" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="21"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A42:A51"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A28:A29"/>
     <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A30:I30"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A30:A37"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
@@ -2600,9 +2546,19 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A9:A16"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A38:A47"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>